<commit_message>
Improving Students’ Satisfaction with the Quality of Innovation and Entrepreneurship Education in Colleges and Universities in the Guangdong-Hong Kong-Macao Greater Bay Area
</commit_message>
<xml_diff>
--- a/slr/ei/data.xlsx
+++ b/slr/ei/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joechan/Documents/development/researchplymouth/slr/ei/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4095CAE-E03D-7B42-8BAA-D95A95E8C11A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52044E1E-D620-4643-B4F0-75C826B6BCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13880" yWindow="3980" windowWidth="35700" windowHeight="27300" xr2:uid="{460A44D5-7B78-304A-AD21-9906C8862B78}"/>
+    <workbookView xWindow="12700" yWindow="11380" windowWidth="35700" windowHeight="27300" xr2:uid="{460A44D5-7B78-304A-AD21-9906C8862B78}"/>
   </bookViews>
   <sheets>
     <sheet name="Consolidated" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3289" uniqueCount="1608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3329" uniqueCount="1648">
   <si>
     <t>#</t>
   </si>
@@ -4923,6 +4923,126 @@
   </si>
   <si>
     <t>This multicountry study empirically explores the institutional determinants of macro-level entrepreneurship. Findings suggest that a society’s normative, cultural-cognitive, and regulative institutions are related to entrepreneurial activity. Normative and cultural-cognitive institutions’ descriptive power in explaining entrepreneurial activity is higher than regulative institutions’ or per capita gross domestic product. This suggests that differences in values, beliefs, and abilities may play a greater role than purely economic considerations of opportunity and transaction costs. Specific attention is given to opportunity- and necessity-motivated entrepreneurship due to their relationship to economic development.</t>
+  </si>
+  <si>
+    <t>To develop a body of evidence-based knowledge on entrepreneurship, findings and contributions from the positivist, narrative, and design research traditions in this area need to be combined. Therefore, a framework for research synthesis in terms of social mechanisms, contextual conditions, and outcome patterns is developed in this paper. Subsequently, a synthesis of the existing body of research findings on entrepreneurial opportunities serves to illustrate how this framework can be applied and provides results that inform entrepreneurial action. Finally, we discuss how this synthetic approach serves to systematically connect the fragmented landscape of entrepreneurship research, and thus gradually build a cumulative and evidence-based body of knowledge on entrepreneurship.</t>
+  </si>
+  <si>
+    <t>This paper studies the role of entrepreneurs in investment tie formation in science-based entrepreneurial firms. Specifically, we address why investment tie formation is path dependent for some firms but more amenable to intentional management for others. Using longitudinal case studies, our evidence suggests that early investment tie formation is path dependent because scientific entrepreneurs typically approach only one or a few prospective investors from within their institutional context. Differences in experience between early investors affect the professionalization of entrepreneurial teams (or lack thereof), which influences the extent to which subsequent investment tie formation becomes more amenable to intentional management or remains path dependent.</t>
+  </si>
+  <si>
+    <t>Entrepreneurial groups face a twinned challenge: recognizing and implementing new ideas. We argue that entrepreneurship is less about importing ideas than about generating new knowledge by recombining resources. In contrast to the brokerage plus closure perspective, we address the overlapping of cohesive group structures. In analyzing the network processes of intercohesion, we identify a distinctive network topology: the structural fold. Actors at the structural fold are multiple insiders, facilitating familiar access to diverse resources. Our data set records personnel ties among the largest 1,696 Hungarian enterprises from 1987 to 2001. First, we test whether structural folding contributes to group performance. Second, because entrepreneurship is a process of generative disruption, we test the contribution of structural folds to group instability. Third, we move from dynamic methods to historical network analysis and demonstrate that coherence is a property of interwoven lineages of cohesion, built up through repeated separation and reunification.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A growing body of scholarship studies the emergence of moral markets— sectors offering market-based solutions to social and environmental issues. To date, researchers have largely focused on the drivers of firm entry into these values-laden sectors. However, we know comparatively little about postentry dynamics or the determinants of firm survival in moral markets. This study examines how regional institutional logics—spatially bound, socially constructed meaning systems that legitimize specific practices and goals within a community—shape firm survival in emerging moral markets. Using a unique panel of firms entering the first eight years of the U.S. green building supply industry, we find that (1) a regional market logic amplifies the impacts of market forces by increasing the positive impact of market adoption and the negative impact of localized competition on firm survival, (2) a regional proenvironmental logic dampens the impacts of adoption and competition on firm survival, and (3) institutional complexity—the co-occurrence of both market and proenvironmental logics in a region—negates the traditional advantages of de alio (diversifying incumbent) firms, creating an opportunity for de novo (entrepreneurial entrant) firms to compete more effectively. Our study integrates research on industry emergence, institutional logics, and firm survival to address important gaps in our knowledge regarding the evolution and growth of environmental entrepreneurship in moral markets. </t>
+  </si>
+  <si>
+    <t>entrepreneurship, social responsibility, sustainability/corporate environmentalism, culture, strategy, organization and management theory, institutional theory, organizational ecology (population ecology), organizational identity and identification</t>
+  </si>
+  <si>
+    <t>While 30 years of entrepreneurial orientation (EO) research has demonstrated that EO provides critical insights into questions of organizational-level strategy and performance, how EO manifests inside organizations has received little attention. Instead of assuming that EO is homogenous, we examine the questions of how and why EO might pervade organizations heterogeneously along three dimensions: vertically across hierarchy levels, horizontally across business units, and temporally as an organization develops. We then present three models for how EO can dynamically pervade organizations and discuss how examining the pervasiveness of EO can further our understanding of entrepreneurship as an organizational phenomenon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drawing on a database of 149 university spin-offs, we investigated the impact of network capability (NC), defined as a firm’s ability to develop and utilize inter-organizational relationships, and entrepreneurial orientation (EO) on organizational performance. Not only do the results suggest that a spin-off’s performance is positively influenced by its NC, but the findings also indicate that a spin-off’s EO fosters competitive advantages. Although no direct relationship is apparent between EO and sales growth, sales per employee, or profit attainment, moderated hierarchical regression analyses reveal that NC strengthens the relationship between EO and spin-off performance. In sum, our research shows that a spin-off’s organizational propensities and processes that enhance innovation, constructive risk taking, and proactiveness in dealing with competitors per se do not enhance growth and secure long-term survival. However, we found that NC moderates the relationship between EO and organizational performance. </t>
+  </si>
+  <si>
+    <t>Entrepreneurial orientation, Network capability, University spin-off, Technology transfer, Academic entrepreneurship</t>
+  </si>
+  <si>
+    <t>This study examines how characteristics of university departments impact students’ selfemployment intentions. We argue that four organizational-level factors (entrepreneurship education, entrepreneurship support programs, industry ties, and research orientation) increase such intentions. Using a data set of 1530 business students and 132 professors at 25 university departments, this study shows that entrepreneurship education and industry ties are related to self-employment intentions only for the males in our sample. A negative effect of the department’s research orientation was found. Our study suggests that the organizational context plays an important but gender-specific role in shaping future entrepreneurs. Implications of our findings are discussed.</t>
+  </si>
+  <si>
+    <t>Entrepreneurial orientation (EO) is a key ingredient for firm success. Nonetheless, an important message from past findings is that simply examining the direct effect of EO on firm performance provides an incomplete picture. Prior studies examined various internal and external factors that influence the EO–performance relationship. However, learning orientation (LO) has been a missing link in the examination of the relationship. Using data from 213 medium-to-large UK firms, this study finds that LO mediates the EO-performance relationship, and the EO–LO–performance link is stronger for prospectors than analyzers. The findings indicate that LO must be in place to maximize the effect of EO on performance, and that LO is an important dimension, along with EO, to distinguish prospectors from analyzers.</t>
+  </si>
+  <si>
+    <t>Amidst the intensified discourse surrounding universities’ societal impact, social innovation and entrepreneurship (SIE) has emerged as a way to refocus universities’ engagement in sustainable development, particularly through their core mission of teaching and learning. Growing interest in SIE education over the decades has led to a proliferation of courses and programs offered in various disciplines by universities worldwide. Nevertheless, scholarly research unpacking the SIE educational processes remains scant and lacks multidisciplinary perspectives. Educators of SIE continue to face challenges in designing curricula and adopting appropriate teaching approaches. This study fills this gap by offering ample empirical evidence based on a documentary analysis of 53 syllabi from 43 distinctive courses accompanied by interviews with the academics responsible for the design of these courses across all eight publicly funded universities in Hong Kong. The analysis identifies multiple patterns within two major themes: the changing scope and positioning of SIE education and the varying orientations of SIE curricula. The findings provide valuable insights and identify areas for further exploration for the design of impactful SIE learning experiences for students. Furthermore, by situating the examination of SIE teaching and learning within the lens of curriculum theory, this study establishes a foundation for future research to undertake systematic and rigorous comparative analyses of curricula in diverse contexts.</t>
+  </si>
+  <si>
+    <t>Entrepreneurship education, social entrepreneurship, social innovation, curriculum theory, higher education</t>
+  </si>
+  <si>
+    <t>In response to society’s growing focus on social and environmental challenges, universities worldwide are integrating social innovation and entrepreneurship (SIE) education into their curricula. This is a vital step towards achieving sustainable development. However, many SIE education initiatives struggle to maintain rigour and long-term sustainability due to inherent tensions within the university system. While the overall trend is promising, it is crucial to examine what underpins the varied development of SIE courses and programmes. Central to this inquiry are academics, whose agentic roles in educational changes have been acknowledged in the literature but remain understudied in the context of SIE education. Addressing this gap, the present study adopts an agent-based perspective to investigate academics’ experiences and perspectives as they design, implement, and drive innovations in SIE education. Drawing on interviews with 30 academics teaching and leading SIE courses and programmes across diverse disciplines and academic positions in Hong Kong’s eight publicly funded universities, the study reveals that their agency emerges through the reflexive processes of aligning motives and navigating structures. The analysis also identifies factors at multiple levels that condition academics’ agency and highlights the heterogeneity of their experiences based on their roles as professoriate, teaching, or practitioner academics. This study deepens understanding of the agency–structure interplay in SIE education, offering insights that can help university leaders and policymakers better support academics engaged in SIE education. The findings also add nuance to interpretations of the global proliferation of SIE programmes and enrich discourse on universities’ societal engagement through teaching.</t>
+  </si>
+  <si>
+    <t>Social innovation and entrepreneurship, higher education, academic agency, social impact, educational change</t>
+  </si>
+  <si>
+    <t>Although base of the pyramid markets are significant sources of entrepreneurial opportunities, the nature of entrepreneurship in these markets is not well understood. Additionally, these markets remain largely underserved by multinational enterprises (MNEs). Given theoretical and practical gaps associated with these issues, we integrate entrepreneurship, institutional, and network theories to discuss how the entrepreneurship process of MNEs is negatively affected in base of the pyramid markets. We then explain how partnerships with nongovernment organizations (NGOs) can offset such negative effects due to NGOs’ high degree of localized knowledge, social embeddedness within multiple informal networks, and ambidexterity in dealing with diverse stakeholder groups. Both economic and social benefits can result from such partnerships.</t>
+  </si>
+  <si>
+    <t>This study illuminates how new markets emerge and how social movements can effect cultural change through market creation. We suggest that social movements can fuel solutions to three challenges in creating new market segments: entrepreneurial production, the creation of collective producer identities, and the establishment of regular exchange between producers and consumers. We use qualitative data on the grassroots coalition movement that has spurred a market for grass-fed meat and dairy products in the United States since the early 1990s. Our analysis shows that the movement's participants mobilized broad cultural codes and that these codes motivated producers to enter and persist in a nascent market, shaped their choices about production and exchange technologies, enabled a collective identity, and formed the basis of the products' exchange value.</t>
+  </si>
+  <si>
+    <t>This research examines the interplay of opportunity evaluation and emotions as determinants of entrepreneurial exploitation using affect-as-information theory and the affective processing principle as conceptual bases. Three central assumptions are confirmed across two studies. The first is that the effects of opportunity characteristics on exploitation are mediated by evaluation. The second is that emotions influence exploitation decisions in addition to evaluation. Fear reduces exploitation, whereas joy and anger increase it. The third is that fear, joy, and anger influence evaluation’s effect on exploitation with higher levels of fear reducing and higher levels of joy and anger increasing the positive impact of evaluation on exploitation.</t>
+  </si>
+  <si>
+    <t>This paper sets out to explore contexts for entrepreneurship, illustrating how a contextualized view of entrepreneurship contributes to our understanding of the phenomenon. There is growing recognition in entrepreneurship research that economic behavior can be better understood within its historical, temporal, institutional, spatial, and social contexts, as these contexts provide individuals with opportunities and set boundaries for their actions. Context can be an asset and a liability for the nature and extent of entrepreneurship, but entrepreneurship can also impact contexts. The paper argues that context is important for understanding when, how, and why entrepreneurship happens and who becomes involved. Exploring the multiplicity of contexts and their impact on entrepreneurship, it identifies challenges researchers face in contextualizing entrepreneurship theory and offers possible ways forward.</t>
+  </si>
+  <si>
+    <t>Designing effective strategies for developing higher education students’ competencies, such as creativity and entrepreneurship, is crucial for their survival and self-realization in the technology-rich 21st century. This study is important as it addresses a significant research gap by designing and implementing self-determination theory (SDT)-guided case-based instruction (CBI) to enhance digital learners’ creativity and entrepreneurship. A class of 34 master’s students in a taught programme focused on digital learning and technology at a public university in Hong Kong participated in the study. First, the students took a pre-test to assess their creativity and entrepreneurship. They then experienced a 13-week course designed using SDT-guided CBI. After the intervention, they completed a post-test on their creativity and entrepreneurship. Additionally, the researchers conducted interviews with 10 participants. These processes allowed the researchers to evaluate the effectiveness of the SDT-guided CBI learning activities and to gather participants’ suggestions for improving the design. The results of a repeated measures analysis of variance indicated the feasibility of SDT-guided CBI. Significant improvements in creativity were observed from the pre-test to the post-test, from the pre-test to the mid-test, and from the mid-test to the post-test. Meanwhile, students’ entrepreneurship significantly increased from the pre-test to the posttest, although the increases from the pre-test to the mid-test and from the mid-test to the post-test were slight and did not reach a significant level. From the qualitative data, students provided suggestions such as selecting effective case studies, using entrepreneurs’ stories, supporting entrepreneurial experiences, promoting technology-enhanced learning, and advocating for collaborative learning to improve the design. The findings imply that SDTguided CBI has the potential to continually enhance students’ creativity and entrepreneurship throughout its implementation, with significant opportunities for improvement based on the implementation experiences.</t>
+  </si>
+  <si>
+    <t>While much prior research has focused upon how the Technology Transfer Offices (TTOs) and other contextual characteristics shape the level of university spinoffs (USO), there is little research on entrepreneurial potential among individual academics, and to the best of our knowledge, no comparative studies with other types of spinoffs exist to date. In this paper we focus on an important but neglected aspect of knowledge transfer from academic research involving the indirect flow to entrepreneurship by individuals with a university education background who become involved in new venture creation by means of corporate spinoffs (CSO) after gaining industrial experience, rather than leaving university employment to found a new venture as an academic spinoff. We argue that the commercial knowledge gained by industry experience is potentially more valuable for entrepreneurial performance compared to the academic knowledge gained by additional research experience at a university. This leads us to posit that the average performance of CSOs will be higher than comparable USOs, but the gains from founder‘s prior experiences will be relatively higher among USOs whose founders lack the corporate context. We investigate these propositions in a comparative study tracking the complete population of USOs and CSOs among the Swedish knowledge-intensive sectors between 1994 and 2002.</t>
+  </si>
+  <si>
+    <t>University spinoffs, Corporate spinoffs, Technology Transfer Offices</t>
+  </si>
+  <si>
+    <t>New venture success often depends on how the founding team collectively understands its world, estimates effects of possible actions, makes decisions, and allocates appropriate resources. Drawing on recent work in managerial cognition and entrepreneurship, this article argues for the importance of examining cognition at the team level. New venture strategy is used as a springboard to discuss collective cognition, although other important critical decision domains in new ventures may also be used to illustrate the arguments. In this and other such decision domains, collective cognition mediates between individual cognitions and firm actions and performance. A method for assessing entrepreneurial top management team cognition is developed and then tested in an exploratory study of technology-based new ventures. Two structural characteristics of collective cognition (differentiation and integration) are strongly related to firm performance, suggesting interesting opportunities for future entrepreneurship research in cognition.</t>
+  </si>
+  <si>
+    <t>Emerging economies face daunting economic development challenges. Economists and management consultants have generally suggested global solutions that typically focus solely on foreign direct investment. Yet a resource-based theory approach offers an alternative view of economic development in which a foundation of resources within a region gestates entrepreneurial activity. While theoretically appealing, it is unclear in application how such resources can be developed or which types of resources are most important to develop. This paper extends the application of resource-based theory to entrepreneurial economic development in subsistence economies. A qualitative study of contrasting entrepreneurial activity in Chiapas (Mexico) and Atenas (Costa Rica) highlights the primacy of intangible resources—and especially entrepreneurial orientation resources—in the gestation of entrepreneurial activity.</t>
+  </si>
+  <si>
+    <t>Venture capitalists (VCs) contribute to entrepreneurial firms by engaging in governance activities, such as providing services and monitoring the entrepreneurial firm’s operations and performance. This study examines the role and influence of the VC’s governance activities on 93 Dutch entrepreneurial firms. Results suggest that while the VC’s governance activities may help to stimulate the use of the entrepreneurial firm’s control systems, they also moderate the relationship between the entrepreneurial firm’s use of control systems and its financial performance. It appears in particular that cost control systems contribute positively to the entrepreneurial firm’s financial performance when the VC provides service activities. However, the use of cost control systems tends to be negatively related to the entrepreneurial firm’s financial performance when the VC is highly focused on monitoring.</t>
+  </si>
+  <si>
+    <t>This article examines two potential causal mechanisms underlying the observed entrepreneurial orientation (EO)–performance relationship. We find empirical support for the notion that EO might be a performance–variance-enhancing strategic orientation rather than a performance–mean-enhancing orientation. With such a conceptualization, performance variance (along with, or instead of, mean performance) and failure take center stage. To address the question of “where to from here,” we discuss a number of research opportunities that we believe are going to make important contributions to the entrepreneurship and strategy literature.</t>
+  </si>
+  <si>
+    <t>The relationships between gender, entrepreneurial self-efficacy, and entrepreneurial intentions were examined for two sample groups: adolescents and adult master of business administration (MBA) students. Similar gender effects on entrepreneurial self-efficacy are shown for both groups and support earlier research on the relationship between self-efficacy and career intentions. Additionally, the effects of entrepreneurship education in MBA programs on entrepreneurial self-efficacy proved stronger for women than for men. Implications for educators and policy makers were discussed, and areas for future research outlined.</t>
+  </si>
+  <si>
+    <t>In this editorial, I seek to inform entrepreneurship scholars about the significance of unequivocal “A” level entrepreneurship journals for the continued ascent of entrepreneurship as a universally recognized “mainstream” academic field. Drawing insights from research on intellectual movements and the evolution of academic fields, I take stock of entrepreneurship as a community of scholars mobilizing elements of distinctiveness and legitimacy to elevate the status of the field. Doing so, I offer three field level observations on the primacy of unequivocal “A” journals for advancing the field. I then delineate a set of role related implications for members of the community, including authors, senior scholars, and newcomers to the field. Finally, I entertain some common objections to emphasizing journal status as a mechanism in entrepreneurship's upsurge to “mainstream” academic field.</t>
+  </si>
+  <si>
+    <t>Entrepreneurship, Academic field, Journal, Community</t>
+  </si>
+  <si>
+    <t>Entrepreneurship is a perilous endeavor. Contextual changes, such as nascent technology emergence or new industry creation, can spawn entrepreneurial opportunities; however, these changes do not instantaneously create the resources and structures that new firms need to survive. This study examines the creation and configuration of the contextual infrastructure necessary for nascent technology entrepreneurship in new industries. Using the case of nanotechnology, I show how the elements of infrastructure emerge and configure through systemic coevolution. The data highlight how boundary crossing and obfuscation induces the configuration of separate elements into a cohesive infrastructure through heightened interaction and interdependence of organizations and institutions, both private and public.</t>
+  </si>
+  <si>
+    <t>This study explores the performance implications of internal resources and external networks for entrepreneurial firms. A relationship of trust among network members is essential because of the high risk during the initial start-up stage. However, once high-tech firms initiate mass production and enter the growth stage, whether trust influences competitiveness more than resources becomes uncertain. This study examines Taiwanese firms to elucidate the main influences on firm competitiveness. In conclusion, the result indicates the competitiveness of high-tech firms during the growth stage is determined by firm resources and the willingness of support firms to cooperate—where willingness is determined by the trust of the support firms in the high-tech firm but is unrelated to firm resources.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This study focuses on exploring the elements needed for entrepreneurship education in the future for generating economic, social and environmental sustainability for the community and for developing future leaders through understanding the existing entrepreneurship related policies, programmes, modules and the perception of teenagers of entrepreneurship skills to realise the importance of a mindset of entrepreneurship and the ways of integrating multidisciplinary knowledge for developing entrepreneurship spirit to meet the challenges of the future. This topic has not been comprehensively explored in the past. After conducting quantitative analysis on 95 undergraduate students of a postsecondary institution in Hong Kong on entrepreneurship skills, the regression results presented in this paper found “entrepreneurship skills include implementation skill” can explain about 33percent of the change in the dependent variable of “sustainable skill sets include building a positive mindset”. And, the mean scores of “entrepreneurship skills include creativity and risk-taking are the same as 4.02 out of a 5-point scale while “dislike handling paperwork with details”, “dislike facing people I don’t know” and “dislike being challenges” received the lowest scores of 2.6, 2.7 and 2.7 respectively. With regard to the qualitative analysis of existing entrepreneurship related programmes, it is found that business, management, finance and contemporary issues are the common elements in existing programmes of which the skills of creativity, risk-taking, socialization, handling details and challenges are lacking. When analysing the meeting notes of UNESCO, APEID in February, 2015 of nine countries (India, Pakistan, Sri Lanka, Indonesia, Malaysia, Philippines, China Hong Kong, Japan, and Republic of Korea), there is a trend on the importance of entrepreneurship and innovation mindset with three common concerns, that is, a lack of competent teachers teaching entrepreneurship programmes, a lack of industry exposure and a lack of government support. This paper highlights the key elements of future entrepreneurship related programmes for sustainability. Both educators and policy makers not only need to respond to the ecosystem of entrepreneurship education, but also need to co-produce relevant and meaningful entrepreneurship related modules and programmes which focus on soft skills development for building a positive mindset for handling challenges of the future. </t>
+  </si>
+  <si>
+    <t>Entrepreneurship Education, Sustainability, Creativity, Risk-Taking, Co-Produce</t>
+  </si>
+  <si>
+    <t>Network-based resource capital such as political capital, social capital, and reputational capital are critical in providing firms with special access to various resources and legitimacy in emerging markets. However, how these generic nonmarket forms of capital are transformed into value-adding, industry-specific, and firm-specific uses, which subsequently enhance firm competitiveness, remained unanswered. Adopting a dynamic capability approach, this paper posits that corporate entrepreneurship performs a unique role of resource capital configuration and transformation in emerging market firms by continuously renewing firm competences so that congruence with the changing environment can be achieved. Building on this conceptualization, we argue that the positive effects of network-based resource capital on firm performance are channeled through the resource configuration process given by various corporate entrepreneurial activities such as product and organizational innovations as well as new venturing. Empirical evidence of the proposed mediation model is obtained from a survey of established firms in China.</t>
+  </si>
+  <si>
+    <t>Universities have assumed an expanded role in science and technology-based economic development that has become of interest to catch-up regions as well as to leading innovation locales. This paper examines how the role of the university has evolved from performing conventional research and education functions to serving as an innovation-promoting knowledge hub though the case of Georgia Institute of Technology (Georgia Tech). This case is discussed in the context of state efforts to shift the region from an agricultural to an industrial to an innovation-driven economy. Central to the transformation of Georgia Tech as a knowledge hub is the emergence of new institutional leadership, programs, organizational forms and boundary-spanning roles that meditate among academic, educational, entrepreneurial, venture capital, industrial, and public spheres. Comparisons between Georgia Tech’s experiences and those of university roles in selected other catch-up regions in the southern United States highlight the importance to the case of networked approaches, capacity building, technology-based entrepreneurial development, and local innovation system leadership. Insights on the transformation of universities and the challenges of fostering a similar transformation in regional economies are offered.</t>
+  </si>
+  <si>
+    <t>Universities, Regional innovation, Tacit knowledge, Boundary spanning</t>
+  </si>
+  <si>
+    <t>Despite extensive though mostly independent literatures on Crowdfunding and regional entrepreneurship, there exists little work that examines how Crowdfunding influences the rate and type of new venture formation in a region, what types of regions are more likely to experience Crowdfunding activity, and what types of regions are more likely to experience additional firm starts following Crowdfunding activity. We argue that Crowdfunding increases high tech and high growth regional firm starts by increasing crucial early-stage funding, providing the opportunity to signal success and legitimacy, facilitating access to entrepreneurial human capital, supporting inexperienced entrepreneurs with education and advice, and providing inexpensive market feedback. Instrumental variable regressions illustrate how Kickstarter campaigns precede an increase in high technology and growth in Crunchbase listings and a weak decrease in more conventional and local business registrations. While more per capita crowdfunding occurs in large cities relative to smaller cities, college towns, and poor regions with weak human capital, the impact per campaign appears greater in the poorer regions.</t>
+  </si>
+  <si>
+    <t>Crowdfunding, Entrepreneurship, Regional economics, Measures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The purpose of this study was to investigate the mediating role of self-efficacy in the development of students’ intentions to become entrepreneurs. The authors used structural equation modeling with a sample of 265 master of business administration students across 5 universities to test their hypotheses. The results showed that the effects of perceived learning from entrepreneurship-related courses, previous entrepreneurial experience, and risk propensity on entrepreneurial intentions were fully mediated by entrepreneurial self-efficacy. Contrary to expectations, gender was not mediated by self-efficacy but had a direct effect such that women reported lower entrepreneurial career intentions. The authors discuss practical implications and directions for future research. </t>
+  </si>
+  <si>
+    <t>entrepreneurship, self-efficacy, career intentions</t>
+  </si>
+  <si>
+    <t>This study examined the relationships among entrepreneurial orientation (EO), experimental learning (EL) and acquisitive learning (AL), and firm performance (FP). We tested our model in China as EO is the engine that is driving firms to take advantage of opportunities in an increasingly market-oriented transitional economy. From the responses of 607 firms, we found that EO was positively related to EL but had an inverse U-shaped relationship with AL. Both EL and AL enhanced FP although the effects from AL were weaker and became nonsignificant when external knowledge was embedded into the firm’s internal private knowledge.</t>
   </si>
 </sst>
 </file>
@@ -5347,8 +5467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1591E0BB-A549-4141-B94E-FC66BB4664AB}">
   <dimension ref="A1:L293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A252" zoomScale="158" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D254" sqref="D254"/>
+    <sheetView tabSelected="1" topLeftCell="A290" zoomScale="158" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D294" sqref="D294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14561,7 +14681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="255" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>1187</v>
       </c>
@@ -14571,6 +14691,9 @@
       <c r="C255" s="3" t="s">
         <v>938</v>
       </c>
+      <c r="D255" s="3" t="s">
+        <v>1608</v>
+      </c>
       <c r="F255" s="3" t="s">
         <v>17</v>
       </c>
@@ -14593,7 +14716,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="256" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>1188</v>
       </c>
@@ -14603,6 +14726,9 @@
       <c r="C256" s="3" t="s">
         <v>941</v>
       </c>
+      <c r="D256" s="3" t="s">
+        <v>1609</v>
+      </c>
       <c r="F256" s="3" t="s">
         <v>17</v>
       </c>
@@ -14625,7 +14751,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="257" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:12" ht="204" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>1189</v>
       </c>
@@ -14635,6 +14761,9 @@
       <c r="C257" s="3" t="s">
         <v>944</v>
       </c>
+      <c r="D257" s="3" t="s">
+        <v>1610</v>
+      </c>
       <c r="F257" s="3" t="s">
         <v>445</v>
       </c>
@@ -14657,7 +14786,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="258" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:12" ht="323" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>1190</v>
       </c>
@@ -14666,6 +14795,12 @@
       </c>
       <c r="C258" s="3" t="s">
         <v>947</v>
+      </c>
+      <c r="D258" s="3" t="s">
+        <v>1611</v>
+      </c>
+      <c r="E258" s="3" t="s">
+        <v>1612</v>
       </c>
       <c r="F258" s="3" t="s">
         <v>10</v>
@@ -14765,7 +14900,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="261" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:12" ht="136" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>1193</v>
       </c>
@@ -14775,6 +14910,9 @@
       <c r="C261" s="3" t="s">
         <v>951</v>
       </c>
+      <c r="D261" s="3" t="s">
+        <v>1613</v>
+      </c>
       <c r="F261" s="3" t="s">
         <v>17</v>
       </c>
@@ -14797,7 +14935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="262" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:12" ht="204" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>1194</v>
       </c>
@@ -14807,6 +14945,12 @@
       <c r="C262" s="3" t="s">
         <v>954</v>
       </c>
+      <c r="D262" s="3" t="s">
+        <v>1614</v>
+      </c>
+      <c r="E262" s="3" t="s">
+        <v>1615</v>
+      </c>
       <c r="F262" s="3" t="s">
         <v>7</v>
       </c>
@@ -14829,7 +14973,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="263" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>1195</v>
       </c>
@@ -14839,6 +14983,9 @@
       <c r="C263" s="3" t="s">
         <v>957</v>
       </c>
+      <c r="D263" s="3" t="s">
+        <v>1616</v>
+      </c>
       <c r="F263" s="3" t="s">
         <v>17</v>
       </c>
@@ -14861,7 +15008,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="264" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>1196</v>
       </c>
@@ -14871,6 +15018,9 @@
       <c r="C264" s="3" t="s">
         <v>960</v>
       </c>
+      <c r="D264" s="3" t="s">
+        <v>1617</v>
+      </c>
       <c r="F264" s="3" t="s">
         <v>17</v>
       </c>
@@ -14893,7 +15043,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="265" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:12" ht="289" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>1343</v>
       </c>
@@ -14903,6 +15053,12 @@
       <c r="C265" s="3" t="s">
         <v>1046</v>
       </c>
+      <c r="D265" s="3" t="s">
+        <v>1618</v>
+      </c>
+      <c r="E265" s="3" t="s">
+        <v>1619</v>
+      </c>
       <c r="F265" s="3" t="s">
         <v>295</v>
       </c>
@@ -14925,7 +15081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="266" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:12" ht="340" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>1344</v>
       </c>
@@ -14935,6 +15091,12 @@
       <c r="C266" s="3" t="s">
         <v>1048</v>
       </c>
+      <c r="D266" s="3" t="s">
+        <v>1620</v>
+      </c>
+      <c r="E266" s="3" t="s">
+        <v>1621</v>
+      </c>
       <c r="F266" s="3" t="s">
         <v>295</v>
       </c>
@@ -14957,7 +15119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="267" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>1197</v>
       </c>
@@ -14967,6 +15129,9 @@
       <c r="C267" s="3" t="s">
         <v>962</v>
       </c>
+      <c r="D267" s="3" t="s">
+        <v>1622</v>
+      </c>
       <c r="F267" s="3" t="s">
         <v>17</v>
       </c>
@@ -14989,7 +15154,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="268" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>1198</v>
       </c>
@@ -14999,6 +15164,9 @@
       <c r="C268" s="3" t="s">
         <v>965</v>
       </c>
+      <c r="D268" s="3" t="s">
+        <v>1623</v>
+      </c>
       <c r="F268" s="3" t="s">
         <v>429</v>
       </c>
@@ -15021,7 +15189,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="269" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:12" ht="136" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>1199</v>
       </c>
@@ -15031,6 +15199,9 @@
       <c r="C269" s="3" t="s">
         <v>968</v>
       </c>
+      <c r="D269" s="3" t="s">
+        <v>1624</v>
+      </c>
       <c r="F269" s="3" t="s">
         <v>17</v>
       </c>
@@ -15053,7 +15224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="270" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>1200</v>
       </c>
@@ -15063,6 +15234,9 @@
       <c r="C270" s="3" t="s">
         <v>971</v>
       </c>
+      <c r="D270" s="3" t="s">
+        <v>1625</v>
+      </c>
       <c r="F270" s="3" t="s">
         <v>17</v>
       </c>
@@ -15085,7 +15259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="271" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:12" ht="388" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>1345</v>
       </c>
@@ -15095,6 +15269,9 @@
       <c r="C271" s="3" t="s">
         <v>1051</v>
       </c>
+      <c r="D271" s="3" t="s">
+        <v>1626</v>
+      </c>
       <c r="F271" s="3" t="s">
         <v>1034</v>
       </c>
@@ -15114,7 +15291,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="272" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:12" ht="272" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>1201</v>
       </c>
@@ -15124,6 +15301,12 @@
       <c r="C272" s="3" t="s">
         <v>974</v>
       </c>
+      <c r="D272" s="3" t="s">
+        <v>1627</v>
+      </c>
+      <c r="E272" s="3" t="s">
+        <v>1628</v>
+      </c>
       <c r="F272" s="3" t="s">
         <v>12</v>
       </c>
@@ -15146,7 +15329,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="273" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:12" ht="204" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>1202</v>
       </c>
@@ -15156,6 +15339,9 @@
       <c r="C273" s="3" t="s">
         <v>977</v>
       </c>
+      <c r="D273" s="3" t="s">
+        <v>1629</v>
+      </c>
       <c r="F273" s="3" t="s">
         <v>17</v>
       </c>
@@ -15178,7 +15364,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="274" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:12" ht="187" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>1203</v>
       </c>
@@ -15188,6 +15374,9 @@
       <c r="C274" s="3" t="s">
         <v>980</v>
       </c>
+      <c r="D274" s="3" t="s">
+        <v>1630</v>
+      </c>
       <c r="F274" s="3" t="s">
         <v>17</v>
       </c>
@@ -15210,7 +15399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="275" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>1204</v>
       </c>
@@ -15220,6 +15409,9 @@
       <c r="C275" s="3" t="s">
         <v>983</v>
       </c>
+      <c r="D275" s="3" t="s">
+        <v>1631</v>
+      </c>
       <c r="F275" s="3" t="s">
         <v>17</v>
       </c>
@@ -15242,7 +15434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="276" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:12" ht="136" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>1205</v>
       </c>
@@ -15252,6 +15444,9 @@
       <c r="C276" s="3" t="s">
         <v>986</v>
       </c>
+      <c r="D276" s="3" t="s">
+        <v>1632</v>
+      </c>
       <c r="F276" s="3" t="s">
         <v>17</v>
       </c>
@@ -15274,7 +15469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="277" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>1206</v>
       </c>
@@ -15283,6 +15478,9 @@
       </c>
       <c r="C277" s="3" t="s">
         <v>989</v>
+      </c>
+      <c r="D277" s="3" t="s">
+        <v>1633</v>
       </c>
       <c r="F277" s="3" t="s">
         <v>17</v>
@@ -15379,7 +15577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="280" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:12" ht="170" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>1208</v>
       </c>
@@ -15389,6 +15587,12 @@
       <c r="C280" s="3" t="s">
         <v>993</v>
       </c>
+      <c r="D280" s="3" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E280" s="3" t="s">
+        <v>1635</v>
+      </c>
       <c r="F280" s="3" t="s">
         <v>7</v>
       </c>
@@ -15411,7 +15615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="281" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>1209</v>
       </c>
@@ -15421,6 +15625,9 @@
       <c r="C281" s="3" t="s">
         <v>996</v>
       </c>
+      <c r="D281" s="3" t="s">
+        <v>1636</v>
+      </c>
       <c r="F281" s="3" t="s">
         <v>17</v>
       </c>
@@ -15443,7 +15650,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="282" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>1210</v>
       </c>
@@ -15453,6 +15660,9 @@
       <c r="C282" s="3" t="s">
         <v>999</v>
       </c>
+      <c r="D282" s="3" t="s">
+        <v>1637</v>
+      </c>
       <c r="F282" s="3" t="s">
         <v>17</v>
       </c>
@@ -15475,7 +15685,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="283" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>1347</v>
       </c>
@@ -15485,6 +15695,12 @@
       <c r="C283" s="3" t="s">
         <v>1055</v>
       </c>
+      <c r="D283" s="3" t="s">
+        <v>1638</v>
+      </c>
+      <c r="E283" s="3" t="s">
+        <v>1639</v>
+      </c>
       <c r="F283" s="3" t="s">
         <v>1056</v>
       </c>
@@ -15501,7 +15717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="284" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:12" ht="221" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>1211</v>
       </c>
@@ -15511,6 +15727,9 @@
       <c r="C284" s="3" t="s">
         <v>1002</v>
       </c>
+      <c r="D284" s="3" t="s">
+        <v>1640</v>
+      </c>
       <c r="F284" s="3" t="s">
         <v>17</v>
       </c>
@@ -15533,7 +15752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="285" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:12" ht="255" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>1212</v>
       </c>
@@ -15543,6 +15762,12 @@
       <c r="C285" s="3" t="s">
         <v>1005</v>
       </c>
+      <c r="D285" s="3" t="s">
+        <v>1641</v>
+      </c>
+      <c r="E285" s="3" t="s">
+        <v>1642</v>
+      </c>
       <c r="F285" s="3" t="s">
         <v>12</v>
       </c>
@@ -15565,7 +15790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="286" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:12" ht="221" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>1213</v>
       </c>
@@ -15574,6 +15799,12 @@
       </c>
       <c r="C286" s="3" t="s">
         <v>1008</v>
+      </c>
+      <c r="D286" s="3" t="s">
+        <v>1643</v>
+      </c>
+      <c r="E286" s="3" t="s">
+        <v>1644</v>
       </c>
       <c r="F286" s="3" t="s">
         <v>12</v>
@@ -15749,7 +15980,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="291" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:12" ht="153" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>1217</v>
       </c>
@@ -15759,6 +15990,12 @@
       <c r="C291" s="3" t="s">
         <v>1011</v>
       </c>
+      <c r="D291" s="3" t="s">
+        <v>1645</v>
+      </c>
+      <c r="E291" s="3" t="s">
+        <v>1646</v>
+      </c>
       <c r="F291" s="3" t="s">
         <v>68</v>
       </c>
@@ -15781,7 +16018,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="292" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>1218</v>
       </c>
@@ -15790,6 +16027,9 @@
       </c>
       <c r="C292" s="3" t="s">
         <v>1014</v>
+      </c>
+      <c r="D292" s="3" t="s">
+        <v>1647</v>
       </c>
       <c r="F292" s="3" t="s">
         <v>17</v>

</xml_diff>